<commit_message>
Updated sumsum and xlsx for new GETCONSTARRAY results
</commit_message>
<xml_diff>
--- a/data/8_16_32_bit.xlsx
+++ b/data/8_16_32_bit.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="42">
   <si>
     <t>REORDERED</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>Fill array</t>
+  </si>
+  <si>
+    <t>UPDATED 20180301</t>
   </si>
 </sst>
 </file>
@@ -157,7 +160,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -179,7 +181,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,6 +206,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -214,7 +222,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -252,15 +260,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -279,6 +298,11 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -297,6 +321,11 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -626,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W30"/>
+  <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:D30"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -954,7 +983,7 @@
         <v>22.5</v>
       </c>
       <c r="I8">
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
       <c r="J8">
         <v>4.5</v>
@@ -984,7 +1013,7 @@
         <v>37.200000000000003</v>
       </c>
       <c r="S8">
-        <v>18</v>
+        <v>17.899999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:23">
@@ -1072,7 +1101,7 @@
         <v>69.599999999999994</v>
       </c>
       <c r="I10">
-        <v>9.9</v>
+        <v>10.4</v>
       </c>
       <c r="J10">
         <v>64.599999999999994</v>
@@ -1102,7 +1131,7 @@
         <v>118.5</v>
       </c>
       <c r="S10">
-        <v>83.1</v>
+        <v>83.2</v>
       </c>
     </row>
     <row r="12" spans="1:23" s="2" customFormat="1">
@@ -1176,47 +1205,47 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:P14" si="0">MATCH(C13,$A$2:$R$2,0)</f>
+        <f>MATCH(C13,$A$2:$R$2,0)</f>
         <v>2</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f>MATCH(D13,$A$2:$R$2,0)</f>
         <v>3</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f>MATCH(E13,$A$2:$R$2,0)</f>
         <v>17</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f>MATCH(F13,$A$2:$R$2,0)</f>
         <v>4</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
+        <f>MATCH(G13,$A$2:$R$2,0)</f>
         <v>5</v>
       </c>
       <c r="H14">
-        <f t="shared" si="0"/>
+        <f>MATCH(H13,$A$2:$R$2,0)</f>
         <v>15</v>
       </c>
       <c r="I14">
-        <f t="shared" si="0"/>
+        <f>MATCH(I13,$A$2:$R$2,0)</f>
         <v>6</v>
       </c>
       <c r="J14">
-        <f t="shared" si="0"/>
+        <f>MATCH(J13,$A$2:$R$2,0)</f>
         <v>7</v>
       </c>
       <c r="K14">
-        <f t="shared" si="0"/>
+        <f>MATCH(K13,$A$2:$R$2,0)</f>
         <v>18</v>
       </c>
       <c r="L14">
-        <f t="shared" si="0"/>
+        <f>MATCH(L13,$A$2:$R$2,0)</f>
         <v>10</v>
       </c>
       <c r="M14">
-        <f t="shared" si="0"/>
+        <f>MATCH(M13,$A$2:$R$2,0)</f>
         <v>11</v>
       </c>
       <c r="N14">
@@ -1228,7 +1257,7 @@
         <v>13</v>
       </c>
       <c r="P14">
-        <f t="shared" si="0"/>
+        <f>MATCH(P13,$A$2:$R$2,0)</f>
         <v>14</v>
       </c>
       <c r="Q14">
@@ -1253,67 +1282,67 @@
         <v>bsort8</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" ref="C15:R20" si="1">INDEX($A$2:$R$10,$W15,C$14)</f>
+        <f>INDEX($A$2:$R$10,$W15,C$14)</f>
         <v>bsort16</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W15,D$14)</f>
         <v>bsort32</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W15,E$14)</f>
         <v>hsort8</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W15,F$14)</f>
         <v>hsort16</v>
       </c>
       <c r="G15" t="str">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W15,G$14)</f>
         <v>hsort32</v>
       </c>
       <c r="H15" t="str">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W15,H$14)</f>
         <v>binsrch8</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W15,I$14)</f>
         <v>binsrch16</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W15,J$14)</f>
         <v>binsrch32</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W15,K$14)</f>
         <v>outlier8u</v>
       </c>
       <c r="L15" t="str">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W15,L$14)</f>
         <v>outlier16u</v>
       </c>
       <c r="M15" t="str">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W15,M$14)</f>
         <v>outlier32u</v>
       </c>
       <c r="N15" t="str">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W15,N$14)</f>
         <v>fillarray8</v>
       </c>
       <c r="O15" t="str">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W15,O$14)</f>
         <v>fillarray16</v>
       </c>
       <c r="P15" t="str">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W15,P$14)</f>
         <v>fillarray32</v>
       </c>
       <c r="Q15" t="str">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W15,Q$14)</f>
         <v>fft8</v>
       </c>
       <c r="R15" t="str">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W15,R$14)</f>
         <v>fft16</v>
       </c>
       <c r="W15">
@@ -1326,71 +1355,71 @@
         <v>total</v>
       </c>
       <c r="B16">
-        <f t="shared" ref="B16:Q20" si="2">INDEX($A$2:$R$10,$W16,B$14)</f>
+        <f>INDEX($A$2:$R$10,$W16,B$14)</f>
         <v>139.5</v>
       </c>
       <c r="C16">
-        <f t="shared" si="2"/>
+        <f>INDEX($A$2:$R$10,$W16,C$14)</f>
         <v>101.2</v>
       </c>
       <c r="D16">
-        <f t="shared" si="2"/>
+        <f>INDEX($A$2:$R$10,$W16,D$14)</f>
         <v>94.4</v>
       </c>
       <c r="E16">
-        <f t="shared" si="2"/>
+        <f>INDEX($A$2:$R$10,$W16,E$14)</f>
         <v>128.4</v>
       </c>
       <c r="F16">
-        <f t="shared" si="2"/>
+        <f>INDEX($A$2:$R$10,$W16,F$14)</f>
         <v>88.5</v>
       </c>
       <c r="G16">
-        <f t="shared" si="2"/>
+        <f>INDEX($A$2:$R$10,$W16,G$14)</f>
         <v>66.2</v>
       </c>
       <c r="H16">
-        <f t="shared" si="2"/>
+        <f>INDEX($A$2:$R$10,$W16,H$14)</f>
         <v>106.3</v>
       </c>
       <c r="I16">
-        <f t="shared" si="2"/>
+        <f>INDEX($A$2:$R$10,$W16,I$14)</f>
         <v>65.2</v>
       </c>
       <c r="J16">
-        <f t="shared" si="2"/>
+        <f>INDEX($A$2:$R$10,$W16,J$14)</f>
         <v>66</v>
       </c>
       <c r="K16">
-        <f t="shared" si="2"/>
+        <f>INDEX($A$2:$R$10,$W16,K$14)</f>
         <v>159</v>
       </c>
       <c r="L16">
-        <f t="shared" si="2"/>
+        <f>INDEX($A$2:$R$10,$W16,L$14)</f>
         <v>75.7</v>
       </c>
       <c r="M16">
-        <f t="shared" si="2"/>
+        <f>INDEX($A$2:$R$10,$W16,M$14)</f>
         <v>121.6</v>
       </c>
       <c r="N16">
-        <f t="shared" si="2"/>
+        <f>INDEX($A$2:$R$10,$W16,N$14)</f>
         <v>210.1</v>
       </c>
       <c r="O16">
-        <f t="shared" si="2"/>
+        <f>INDEX($A$2:$R$10,$W16,O$14)</f>
         <v>182.8</v>
       </c>
       <c r="P16">
-        <f t="shared" si="2"/>
+        <f>INDEX($A$2:$R$10,$W16,P$14)</f>
         <v>155.30000000000001</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="2"/>
+        <f>INDEX($A$2:$R$10,$W16,Q$14)</f>
         <v>96.7</v>
       </c>
       <c r="R16">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W16,R$14)</f>
         <v>17.7</v>
       </c>
       <c r="W16">
@@ -1403,71 +1432,71 @@
         <v>push/pop</v>
       </c>
       <c r="B17">
-        <f t="shared" si="2"/>
+        <f>INDEX($A$2:$R$10,$W17,B$14)</f>
         <v>0</v>
       </c>
       <c r="C17">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W17,C$14)</f>
         <v>0</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W17,D$14)</f>
         <v>0</v>
       </c>
       <c r="E17">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W17,E$14)</f>
         <v>1.9</v>
       </c>
       <c r="F17">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W17,F$14)</f>
         <v>-2.8</v>
       </c>
       <c r="G17">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W17,G$14)</f>
         <v>-7</v>
       </c>
       <c r="H17">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W17,H$14)</f>
         <v>0</v>
       </c>
       <c r="I17">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W17,I$14)</f>
         <v>0</v>
       </c>
       <c r="J17">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W17,J$14)</f>
         <v>0</v>
       </c>
       <c r="K17">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W17,K$14)</f>
         <v>-0.3</v>
       </c>
       <c r="L17">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W17,L$14)</f>
         <v>-0.2</v>
       </c>
       <c r="M17">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W17,M$14)</f>
         <v>-0.1</v>
       </c>
       <c r="N17">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W17,N$14)</f>
         <v>-0.8</v>
       </c>
       <c r="O17">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W17,O$14)</f>
         <v>-0.6</v>
       </c>
       <c r="P17">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W17,P$14)</f>
         <v>-0.4</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W17,Q$14)</f>
         <v>0</v>
       </c>
       <c r="R17">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W17,R$14)</f>
         <v>2</v>
       </c>
       <c r="W17">
@@ -1480,72 +1509,72 @@
         <v>load/store</v>
       </c>
       <c r="B18">
-        <f t="shared" si="2"/>
+        <f>INDEX($A$2:$R$10,$W18,B$14)</f>
         <v>1.5</v>
       </c>
       <c r="C18">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W18,C$14)</f>
         <v>1</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W18,D$14)</f>
         <v>9</v>
       </c>
       <c r="E18">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W18,E$14)</f>
         <v>32.700000000000003</v>
       </c>
       <c r="F18">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W18,F$14)</f>
         <v>29.3</v>
       </c>
       <c r="G18">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W18,G$14)</f>
         <v>33.200000000000003</v>
       </c>
       <c r="H18">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W18,H$14)</f>
         <v>36.4</v>
       </c>
       <c r="I18">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W18,I$14)</f>
         <v>27</v>
       </c>
       <c r="J18">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W18,J$14)</f>
         <v>33.200000000000003</v>
       </c>
       <c r="K18">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W18,K$14)</f>
         <v>37.200000000000003</v>
       </c>
       <c r="L18">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W18,L$14)</f>
         <v>4.5</v>
       </c>
       <c r="M18">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W18,M$14)</f>
         <v>33.799999999999997</v>
       </c>
       <c r="N18">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W18,N$14)</f>
         <v>0.5</v>
       </c>
       <c r="O18">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W18,O$14)</f>
         <v>0.4</v>
       </c>
       <c r="P18">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W18,P$14)</f>
         <v>0.3</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W18,Q$14)</f>
         <v>22.5</v>
       </c>
       <c r="R18">
-        <f t="shared" si="1"/>
-        <v>2.8</v>
+        <f>INDEX($A$2:$R$10,$W18,R$14)</f>
+        <v>2.4</v>
       </c>
       <c r="W18">
         <v>7</v>
@@ -1557,71 +1586,71 @@
         <v>mov(w)</v>
       </c>
       <c r="B19">
-        <f t="shared" si="2"/>
+        <f>INDEX($A$2:$R$10,$W19,B$14)</f>
         <v>14.2</v>
       </c>
       <c r="C19">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W19,C$14)</f>
         <v>10</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W19,D$14)</f>
         <v>10.4</v>
       </c>
       <c r="E19">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W19,E$14)</f>
         <v>6.9</v>
       </c>
       <c r="F19">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W19,F$14)</f>
         <v>9.4</v>
       </c>
       <c r="G19">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W19,G$14)</f>
         <v>3.9</v>
       </c>
       <c r="H19">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W19,H$14)</f>
         <v>14.7</v>
       </c>
       <c r="I19">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W19,I$14)</f>
         <v>11.8</v>
       </c>
       <c r="J19">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W19,J$14)</f>
         <v>11.6</v>
       </c>
       <c r="K19">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W19,K$14)</f>
         <v>3.7</v>
       </c>
       <c r="L19">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W19,L$14)</f>
         <v>6.8</v>
       </c>
       <c r="M19">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W19,M$14)</f>
         <v>17.3</v>
       </c>
       <c r="N19">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W19,N$14)</f>
         <v>16.100000000000001</v>
       </c>
       <c r="O19">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W19,O$14)</f>
         <v>12.1</v>
       </c>
       <c r="P19">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W19,P$14)</f>
         <v>8.1</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W19,Q$14)</f>
         <v>4.5999999999999996</v>
       </c>
       <c r="R19">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W19,R$14)</f>
         <v>2.9</v>
       </c>
       <c r="W19">
@@ -1634,72 +1663,72 @@
         <v>vm+other</v>
       </c>
       <c r="B20">
-        <f t="shared" si="2"/>
+        <f>INDEX($A$2:$R$10,$W20,B$14)</f>
         <v>123.8</v>
       </c>
       <c r="C20">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W20,C$14)</f>
         <v>90.2</v>
       </c>
       <c r="D20">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W20,D$14)</f>
         <v>75.099999999999994</v>
       </c>
       <c r="E20">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W20,E$14)</f>
         <v>87</v>
       </c>
       <c r="F20">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W20,F$14)</f>
         <v>52.5</v>
       </c>
       <c r="G20">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W20,G$14)</f>
         <v>36.1</v>
       </c>
       <c r="H20">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W20,H$14)</f>
         <v>55.3</v>
       </c>
       <c r="I20">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W20,I$14)</f>
         <v>26.4</v>
       </c>
       <c r="J20">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W20,J$14)</f>
         <v>21.2</v>
       </c>
       <c r="K20">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W20,K$14)</f>
         <v>118.5</v>
       </c>
       <c r="L20">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W20,L$14)</f>
         <v>64.599999999999994</v>
       </c>
       <c r="M20">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W20,M$14)</f>
         <v>70.599999999999994</v>
       </c>
       <c r="N20">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W20,N$14)</f>
         <v>194.3</v>
       </c>
       <c r="O20">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W20,O$14)</f>
         <v>170.8</v>
       </c>
       <c r="P20">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W20,P$14)</f>
         <v>147.30000000000001</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="1"/>
+        <f>INDEX($A$2:$R$10,$W20,Q$14)</f>
         <v>69.599999999999994</v>
       </c>
       <c r="R20">
-        <f t="shared" si="1"/>
-        <v>9.9</v>
+        <f>INDEX($A$2:$R$10,$W20,R$14)</f>
+        <v>10.4</v>
       </c>
       <c r="W20">
         <v>9</v>
@@ -1733,11 +1762,11 @@
         <v>139.5</v>
       </c>
       <c r="C25" s="4">
-        <f t="shared" ref="C25:D25" si="3">C16</f>
+        <f t="shared" ref="C25:D25" si="0">C16</f>
         <v>101.2</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>94.4</v>
       </c>
     </row>
@@ -1750,11 +1779,11 @@
         <v>128.4</v>
       </c>
       <c r="C26" s="4">
-        <f t="shared" ref="C26:D26" si="4">F16</f>
+        <f t="shared" ref="C26:D26" si="1">F16</f>
         <v>88.5</v>
       </c>
       <c r="D26" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>66.2</v>
       </c>
     </row>
@@ -1767,11 +1796,11 @@
         <v>106.3</v>
       </c>
       <c r="C27" s="4">
-        <f t="shared" ref="C27:D27" si="5">I16</f>
+        <f t="shared" ref="C27:D27" si="2">I16</f>
         <v>65.2</v>
       </c>
       <c r="D27" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>66</v>
       </c>
     </row>
@@ -1784,11 +1813,11 @@
         <v>159</v>
       </c>
       <c r="C28" s="4">
-        <f t="shared" ref="C28:D28" si="6">L16</f>
+        <f t="shared" ref="C28:D28" si="3">L16</f>
         <v>75.7</v>
       </c>
       <c r="D28" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>121.6</v>
       </c>
     </row>
@@ -1801,11 +1830,11 @@
         <v>210.1</v>
       </c>
       <c r="C29" s="4">
-        <f t="shared" ref="C29:D29" si="7">O16</f>
+        <f t="shared" ref="C29:D29" si="4">O16</f>
         <v>182.8</v>
       </c>
       <c r="D29" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>155.30000000000001</v>
       </c>
     </row>
@@ -1822,6 +1851,11 @@
         <v>17.7</v>
       </c>
       <c r="D30" s="4"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated all sumsum.txt and excel files
</commit_message>
<xml_diff>
--- a/data/8_16_32_bit.xlsx
+++ b/data/8_16_32_bit.xlsx
@@ -144,7 +144,7 @@
     <t>Fill array</t>
   </si>
   <si>
-    <t>UPDATED 20180305</t>
+    <t>UPDATED 20180326</t>
   </si>
 </sst>
 </file>
@@ -208,7 +208,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF6600"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -222,8 +222,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -281,7 +283,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -306,6 +308,7 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -330,6 +333,7 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -662,7 +666,7 @@
   <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>